<commit_message>
Tested all current commands, all working
</commit_message>
<xml_diff>
--- a/lib/db/output_directory/All Expenses.xlsx
+++ b/lib/db/output_directory/All Expenses.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -570,65 +570,65 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>For finally.</t>
+          <t>Tend player.</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>89.42</v>
+        <v>6.3</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Housing</t>
         </is>
       </c>
       <c r="D8" s="2" t="n">
-        <v>44981</v>
+        <v>45101</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Tend player.</t>
+          <t>Trade evidence.</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>6.3</v>
+        <v>19.41</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Housing</t>
+          <t>Utilities</t>
         </is>
       </c>
       <c r="D9" s="2" t="n">
-        <v>45101</v>
+        <v>43854</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Trade evidence.</t>
+          <t>Yourself.</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>19.41</v>
+        <v>43.9</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="D10" s="2" t="n">
-        <v>43854</v>
+        <v>44827</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Yourself.</t>
+          <t>Type big.</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>43.9</v>
+        <v>9.460000000000001</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -636,53 +636,53 @@
         </is>
       </c>
       <c r="D11" s="2" t="n">
-        <v>44827</v>
+        <v>44701</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Type big.</t>
+          <t>Place try.</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9.460000000000001</v>
+        <v>24.71</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Housing</t>
         </is>
       </c>
       <c r="D12" s="2" t="n">
-        <v>44701</v>
+        <v>44038</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Place try.</t>
+          <t>Anything.</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>24.71</v>
+        <v>59.37</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Housing</t>
+          <t>Utilities</t>
         </is>
       </c>
       <c r="D13" s="2" t="n">
-        <v>44038</v>
+        <v>45092</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Anything.</t>
+          <t>Cover low.</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>59.37</v>
+        <v>14.91</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -690,61 +690,61 @@
         </is>
       </c>
       <c r="D14" s="2" t="n">
-        <v>45092</v>
+        <v>44406</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Cover low.</t>
+          <t>Dog movement.</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>14.91</v>
+        <v>65.38</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Utilities</t>
+          <t>Gifts</t>
         </is>
       </c>
       <c r="D15" s="2" t="n">
-        <v>44406</v>
+        <v>44182</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Dog movement.</t>
+          <t>Small.</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>65.38</v>
+        <v>97.97</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Gifts</t>
+          <t>Housing</t>
         </is>
       </c>
       <c r="D16" s="2" t="n">
-        <v>44182</v>
+        <v>44747</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Small.</t>
+          <t>Date night</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>97.97</v>
+        <v>120</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Housing</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="D17" s="2" t="n">
-        <v>44747</v>
+        <v>45121</v>
       </c>
     </row>
     <row r="18">
@@ -768,47 +768,47 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Date night</t>
+          <t>Dinner with friends</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>120</v>
+        <v>45.6</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Food</t>
         </is>
       </c>
       <c r="D19" s="2" t="n">
-        <v>45121</v>
+        <v>45110</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Dinner with friends</t>
+          <t>Gift for brother</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>45.6</v>
+        <v>35.55</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>Gifts</t>
         </is>
       </c>
       <c r="D20" s="2" t="n">
-        <v>45110</v>
+        <v>45127</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Gift for brother</t>
+          <t>Gift for mom</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>35.55</v>
+        <v>45</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
@@ -816,35 +816,35 @@
         </is>
       </c>
       <c r="D21" s="2" t="n">
-        <v>45127</v>
+        <v>45128</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Gift for mom</t>
+          <t>Flight to Denver</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>45</v>
+        <v>350.75</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Gifts</t>
+          <t>Travel</t>
         </is>
       </c>
       <c r="D22" s="2" t="n">
-        <v>45128</v>
+        <v>45021</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Flight to Denver</t>
+          <t>Denver hotel</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>350.75</v>
+        <v>400</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
@@ -852,21 +852,21 @@
         </is>
       </c>
       <c r="D23" s="2" t="n">
-        <v>45021</v>
+        <v>45050</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Denver hotel</t>
+          <t>Denver Air BnB</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>400</v>
+        <v>100</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Travel</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="D24" s="2" t="n">
@@ -876,87 +876,87 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Denver Air BnB</t>
+          <t>Vet bill</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>100</v>
+        <v>75.59999999999999</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Pets</t>
         </is>
       </c>
       <c r="D25" s="2" t="n">
-        <v>45050</v>
+        <v>45128</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Vet bill</t>
+          <t>New computer</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>75.59999999999999</v>
+        <v>500</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Pets</t>
+          <t>Personal</t>
         </is>
       </c>
       <c r="D26" s="2" t="n">
-        <v>45128</v>
+        <v>45100</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>New computer</t>
+          <t>Movie night</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>500</v>
+        <v>35</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Personal</t>
+          <t>Entertainment</t>
         </is>
       </c>
       <c r="D27" s="2" t="n">
-        <v>45100</v>
+        <v>45067</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Movie night</t>
+          <t>Test</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Entertainment</t>
+          <t>Pets</t>
         </is>
       </c>
       <c r="D28" s="2" t="n">
-        <v>45067</v>
+        <v>45128</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Test</t>
+          <t>Ferry ride</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>120</v>
+        <v>10</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Pets</t>
+          <t>Transportation</t>
         </is>
       </c>
       <c r="D29" s="2" t="n">
@@ -966,43 +966,43 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Ferry ride</t>
+          <t>Coffee run</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Transportation</t>
+          <t>Food</t>
         </is>
       </c>
       <c r="D30" s="2" t="n">
-        <v>45128</v>
+        <v>45110</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Coffee run</t>
+          <t>Yard plants</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>13</v>
+        <v>56.75</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>Personal</t>
         </is>
       </c>
       <c r="D31" s="2" t="n">
-        <v>45110</v>
+        <v>45019</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Yard plants</t>
+          <t>New plants for yard</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -1014,25 +1014,43 @@
         </is>
       </c>
       <c r="D32" s="2" t="n">
-        <v>45019</v>
+        <v>45050</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>New plants for yard</t>
+          <t>March water bill</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>56.75</v>
+        <v>34.65</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Personal</t>
+          <t>Utilities</t>
         </is>
       </c>
       <c r="D33" s="2" t="n">
-        <v>45050</v>
+        <v>45017</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>February Water Bill</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>31.9</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Utilities</t>
+        </is>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>44986</v>
       </c>
     </row>
   </sheetData>

</xml_diff>